<commit_message>
Update Code Reduce the error in the calculation of processing time
</commit_message>
<xml_diff>
--- a/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingTimeResult.xlsx
+++ b/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingTimeResult.xlsx
@@ -607,19 +607,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>998</c:v>
+                  <c:v>1002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>900</c:v>
+                  <c:v>892</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>757</c:v>
+                  <c:v>768</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>669</c:v>
+                  <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>617</c:v>
+                  <c:v>628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,8 +650,8 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1895622928"/>
-        <c:axId val="1895615856"/>
+        <c:axId val="1074259264"/>
+        <c:axId val="1074262528"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -883,7 +883,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1895622928"/>
+        <c:axId val="1074259264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1895615856"/>
+        <c:crossAx val="1074262528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -964,7 +964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1895615856"/>
+        <c:axId val="1074262528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1045,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1895622928"/>
+        <c:crossAx val="1074259264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2167,7 +2167,7 @@
         <v>1003</v>
       </c>
       <c r="J3" s="1">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="L3" s="1">
         <v>3</v>
@@ -2281,7 +2281,7 @@
         <v>898</v>
       </c>
       <c r="J4" s="1">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="L4" s="1">
         <v>4</v>
@@ -2395,7 +2395,7 @@
         <v>754</v>
       </c>
       <c r="J5" s="1">
-        <v>757</v>
+        <v>768</v>
       </c>
       <c r="L5" s="1">
         <v>5</v>
@@ -2509,7 +2509,7 @@
         <v>658</v>
       </c>
       <c r="J6" s="1">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="L6" s="1">
         <v>6</v>
@@ -2623,7 +2623,7 @@
         <v>619</v>
       </c>
       <c r="J7" s="1">
-        <v>617</v>
+        <v>628</v>
       </c>
       <c r="L7" s="1">
         <v>7</v>

</xml_diff>

<commit_message>
Add kosarak test result
</commit_message>
<xml_diff>
--- a/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingTimeResult.xlsx
+++ b/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingTimeResult.xlsx
@@ -652,8 +652,8 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1499769520"/>
-        <c:axId val="1499758096"/>
+        <c:axId val="-1258302960"/>
+        <c:axId val="-1258308944"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -885,7 +885,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1499769520"/>
+        <c:axId val="-1258302960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,7 +958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1499758096"/>
+        <c:crossAx val="-1258308944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -966,7 +966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1499758096"/>
+        <c:axId val="-1258308944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +1047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1499769520"/>
+        <c:crossAx val="-1258302960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>